<commit_message>
Adding Tahquitz Jan 2017
</commit_message>
<xml_diff>
--- a/events/Tahquitz_Jan_2017/Tahquitz-Jan-2017.xlsx
+++ b/events/Tahquitz_Jan_2017/Tahquitz-Jan-2017.xlsx
@@ -7,14 +7,18 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Finances" sheetId="1" r:id="rId1"/>
+    <sheet name="Attendees" sheetId="2" r:id="rId1"/>
+    <sheet name="Finances" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Attendees!$A$1:$G$29</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -44,15 +48,147 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Joshua Dang</t>
+  </si>
+  <si>
+    <t>Perm Slip</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Tahquitz</t>
+  </si>
+  <si>
+    <t>Winter Campout</t>
+  </si>
+  <si>
+    <t>Jan 20 - 22, 2017</t>
+  </si>
+  <si>
+    <t>Vincent Pierlot</t>
+  </si>
+  <si>
+    <t>310-828-9913</t>
+  </si>
+  <si>
+    <t>Austin Hargis</t>
+  </si>
+  <si>
+    <t>Jared Arita</t>
+  </si>
+  <si>
+    <t>Justin Arita</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Jared Minear</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>Evan MacLean</t>
+  </si>
+  <si>
+    <t>Simon Pauly</t>
+  </si>
+  <si>
+    <t>John Paul Pauly</t>
+  </si>
+  <si>
+    <t>Dion Cleghorn-Roer</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>Christopher Lavallee</t>
+  </si>
+  <si>
+    <t>Mason Labow</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>714-326-3314</t>
+  </si>
+  <si>
+    <t>Jack Hargis</t>
+  </si>
+  <si>
+    <t>Dan Minear</t>
+  </si>
+  <si>
+    <t>Robert MacLean</t>
+  </si>
+  <si>
+    <t>Mark Pauly</t>
+  </si>
+  <si>
+    <t>Dan Lavallee</t>
+  </si>
+  <si>
+    <t>Adult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -79,9 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +526,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>15</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +819,7 @@
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42675</v>
       </c>
@@ -438,6 +857,10 @@
       </c>
       <c r="F2" t="s">
         <v>9</v>
+      </c>
+      <c r="G2">
+        <f>25 * 5 / 2</f>
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>